<commit_message>
Output format works OK now
</commit_message>
<xml_diff>
--- a/data/example.xlsx
+++ b/data/example.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
+  <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView activeTab="0" windowWidth="19200" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -17,19 +12,21 @@
     <sheet name="EUR" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base!$H$11:$P$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
+    <definedName name="_FilterDatabase" localSheetId="0">Base!$H$11:$P$38</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Base"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"USD"</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"EUR"</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
+  <webPublishing allowPng="1" css="0" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34" count="34">
   <si>
     <t>Empresa</t>
   </si>
@@ -94,34 +91,40 @@
     <t>ORGANIZATION</t>
   </si>
   <si>
+    <t> JPMRUS31 178992312   017323232</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>DANIEL MORONTA TOTAL</t>
+  </si>
+  <si>
+    <t>DANIEL CRESPI COMPANY LIMITED</t>
+  </si>
+  <si>
+    <t>ACCOUNT NUMBER: 9003004000 IBAN: DE800912341230123012 SWIFT: SHQDE33 INTERMEDIARY BANK: BBVA FRANCES CHICAGO BRANCH SWIFT: BBVAUS33 ACCT: 33221123</t>
+  </si>
+  <si>
+    <t>100000000QQ</t>
+  </si>
+  <si>
+    <t>DANIEL CRESPI COMPANY LIMITED TOTAL</t>
+  </si>
+  <si>
+    <t>MICAELA CRESPI COMPANY</t>
+  </si>
+  <si>
+    <t>INTERM BANK: STANICIO'S BANK NEW YORK BRANCH JPMRUS31 BENEFICIARY BANK BBVA FRANCES ARGENTINA BFRPARBA CBU: 1230012301230123 // BENEFICIARY NAME: MICAELA CRESPI COMPANY LTD.</t>
+  </si>
+  <si>
+    <t>MICAELA CRESPI COMPANY TOTAL</t>
+  </si>
+  <si>
     <t>MORSUS33  178992312   017323232</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>DANIEL MORONTA TOTAL</t>
-  </si>
-  <si>
-    <t>DANIEL CRESPI COMPANY LIMITED</t>
-  </si>
-  <si>
-    <t>ACCOUNT NUMBER: 9003004000 IBAN: DE800912341230123012 SWIFT: SHQDE33 INTERMEDIARY BANK: BBVA FRANCES CHICAGO BRANCH SWIFT: BBVAUS33 ACCT: 33221123</t>
-  </si>
-  <si>
-    <t>100000000QQ</t>
-  </si>
-  <si>
-    <t>DANIEL CRESPI COMPANY LIMITED TOTAL</t>
-  </si>
-  <si>
-    <t>MICAELA CRESPI COMPANY</t>
-  </si>
-  <si>
     <t>INTERM BANK: STANICIO'S BANK NEW YORK BRANCH STANUS33 BENEFICIARY BANK BBVA FRANCES ARGENTINA BBVAARBA CBU: 1230012301230123 // BENEFICIARY NAME: MICAELA CRESPI COMPANY LTD.</t>
-  </si>
-  <si>
-    <t>MICAELA CRESPI COMPANY TOTAL</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -130,14 +133,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <u val="none"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
+      <vertAlign val="baseline"/>
+      <sz val="10"/>
+      <strike val="0"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <u val="none"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <vertAlign val="baseline"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,369 +165,72 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+    <border diagonalUp="0" diagonalDown="0">
+      <left style="none">
+        <color rgb="FFC7C7C7"/>
+      </left>
+      <right style="none">
+        <color rgb="FFC7C7C7"/>
+      </right>
+      <top style="none">
+        <color rgb="FFC7C7C7"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FFC7C7C7"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="14" xfId="0">
+      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="B11:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="B1" workbookViewId="0" tabSelected="1">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="1" width="9.142307692307693" hidden="1"/>
+    <col min="2" max="2" style="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" style="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" style="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" style="1" width="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" style="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" style="1" width="12.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" style="1" width="29.855468749999996" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" style="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" style="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" style="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" style="1" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" style="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" style="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" style="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" style="1" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:16" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -552,7 +271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16">
       <c r="B12">
         <v>8</v>
       </c>
@@ -580,10 +299,10 @@
       <c r="L12" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N12" s="1">
+      <c r="M12" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N12" s="2">
         <v>43301</v>
       </c>
       <c r="O12" t="s">
@@ -593,7 +312,7 @@
         <v>-2000</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16">
       <c r="B13">
         <v>8</v>
       </c>
@@ -621,10 +340,10 @@
       <c r="L13" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N13" s="1">
+      <c r="M13" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N13" s="2">
         <v>43301</v>
       </c>
       <c r="O13" t="s">
@@ -634,7 +353,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16">
       <c r="H14" t="s">
         <v>18</v>
       </c>
@@ -643,7 +362,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16">
       <c r="B15">
         <v>10009</v>
       </c>
@@ -671,10 +390,10 @@
       <c r="L15" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N15" s="1">
+      <c r="M15" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N15" s="2">
         <v>43301</v>
       </c>
       <c r="O15" t="s">
@@ -684,7 +403,7 @@
         <v>-200000</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16">
       <c r="B16">
         <v>10009</v>
       </c>
@@ -712,10 +431,10 @@
       <c r="L16" t="s">
         <v>21</v>
       </c>
-      <c r="M16" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N16" s="1">
+      <c r="M16" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N16" s="2">
         <v>43301</v>
       </c>
       <c r="O16" t="s">
@@ -725,7 +444,7 @@
         <v>-200000</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16">
       <c r="H17" t="s">
         <v>23</v>
       </c>
@@ -734,7 +453,7 @@
         <v>-400000</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16">
       <c r="B18">
         <v>3400</v>
       </c>
@@ -759,10 +478,10 @@
       <c r="L18" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N18" s="1">
+      <c r="M18" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N18" s="2">
         <v>43301</v>
       </c>
       <c r="O18" t="s">
@@ -772,7 +491,7 @@
         <v>-200000</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16">
       <c r="B19">
         <v>3400</v>
       </c>
@@ -797,10 +516,10 @@
       <c r="L19" t="s">
         <v>25</v>
       </c>
-      <c r="M19" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N19" s="1">
+      <c r="M19" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N19" s="2">
         <v>43301</v>
       </c>
       <c r="O19" t="s">
@@ -810,7 +529,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16">
       <c r="B20">
         <v>3400</v>
       </c>
@@ -835,10 +554,10 @@
       <c r="L20" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N20" s="1">
+      <c r="M20" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N20" s="2">
         <v>43301</v>
       </c>
       <c r="O20" t="s">
@@ -848,7 +567,7 @@
         <v>-300000</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16">
       <c r="B21">
         <v>3400</v>
       </c>
@@ -873,10 +592,10 @@
       <c r="L21" t="s">
         <v>25</v>
       </c>
-      <c r="M21" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N21" s="1">
+      <c r="M21" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N21" s="2">
         <v>43301</v>
       </c>
       <c r="O21" t="s">
@@ -886,7 +605,7 @@
         <v>-2300</v>
       </c>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16">
       <c r="B22">
         <v>3400</v>
       </c>
@@ -911,10 +630,10 @@
       <c r="L22" t="s">
         <v>25</v>
       </c>
-      <c r="M22" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N22" s="1">
+      <c r="M22" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N22" s="2">
         <v>43301</v>
       </c>
       <c r="O22" t="s">
@@ -924,7 +643,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16">
       <c r="B23">
         <v>3400</v>
       </c>
@@ -949,10 +668,10 @@
       <c r="L23" t="s">
         <v>25</v>
       </c>
-      <c r="M23" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N23" s="1">
+      <c r="M23" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N23" s="2">
         <v>43301</v>
       </c>
       <c r="O23" t="s">
@@ -962,7 +681,7 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16">
       <c r="B24">
         <v>3400</v>
       </c>
@@ -987,10 +706,10 @@
       <c r="L24" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N24" s="1">
+      <c r="M24" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N24" s="2">
         <v>43301</v>
       </c>
       <c r="O24" t="s">
@@ -1000,7 +719,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16">
       <c r="B25">
         <v>3400</v>
       </c>
@@ -1025,10 +744,10 @@
       <c r="L25" t="s">
         <v>25</v>
       </c>
-      <c r="M25" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N25" s="1">
+      <c r="M25" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N25" s="2">
         <v>43301</v>
       </c>
       <c r="O25" t="s">
@@ -1038,7 +757,7 @@
         <v>12220</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16">
       <c r="B26">
         <v>3400</v>
       </c>
@@ -1063,10 +782,10 @@
       <c r="L26" t="s">
         <v>25</v>
       </c>
-      <c r="M26" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N26" s="1">
+      <c r="M26" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N26" s="2">
         <v>43301</v>
       </c>
       <c r="O26" t="s">
@@ -1076,7 +795,7 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16">
       <c r="B27">
         <v>3400</v>
       </c>
@@ -1101,10 +820,10 @@
       <c r="L27" t="s">
         <v>25</v>
       </c>
-      <c r="M27" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N27" s="1">
+      <c r="M27" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N27" s="2">
         <v>43301</v>
       </c>
       <c r="O27" t="s">
@@ -1114,7 +833,7 @@
         <v>-4000000</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16">
       <c r="B28">
         <v>3400</v>
       </c>
@@ -1139,10 +858,10 @@
       <c r="L28" t="s">
         <v>25</v>
       </c>
-      <c r="M28" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N28" s="1">
+      <c r="M28" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N28" s="2">
         <v>43301</v>
       </c>
       <c r="O28" t="s">
@@ -1152,7 +871,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16">
       <c r="B29">
         <v>3400</v>
       </c>
@@ -1177,10 +896,10 @@
       <c r="L29" t="s">
         <v>25</v>
       </c>
-      <c r="M29" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N29" s="1">
+      <c r="M29" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N29" s="2">
         <v>43301</v>
       </c>
       <c r="O29" t="s">
@@ -1190,7 +909,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16">
       <c r="B30">
         <v>3400</v>
       </c>
@@ -1215,10 +934,10 @@
       <c r="L30" t="s">
         <v>25</v>
       </c>
-      <c r="M30" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N30" s="1">
+      <c r="M30" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N30" s="2">
         <v>43301</v>
       </c>
       <c r="O30" t="s">
@@ -1228,7 +947,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16">
       <c r="B31">
         <v>3400</v>
       </c>
@@ -1253,10 +972,10 @@
       <c r="L31" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N31" s="1">
+      <c r="M31" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N31" s="2">
         <v>43301</v>
       </c>
       <c r="O31" t="s">
@@ -1266,7 +985,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16">
       <c r="H32" t="s">
         <v>27</v>
       </c>
@@ -1275,7 +994,7 @@
         <v>-4555112</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16">
       <c r="B33">
         <v>2020</v>
       </c>
@@ -1300,10 +1019,10 @@
       <c r="L33" t="s">
         <v>29</v>
       </c>
-      <c r="M33" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N33" s="1">
+      <c r="M33" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N33" s="2">
         <v>43301</v>
       </c>
       <c r="O33" t="s">
@@ -1313,7 +1032,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16">
       <c r="B34">
         <v>2020</v>
       </c>
@@ -1338,10 +1057,10 @@
       <c r="L34" t="s">
         <v>29</v>
       </c>
-      <c r="M34" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N34" s="1">
+      <c r="M34" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N34" s="2">
         <v>43301</v>
       </c>
       <c r="O34" t="s">
@@ -1351,7 +1070,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16">
       <c r="B35">
         <v>2020</v>
       </c>
@@ -1376,10 +1095,10 @@
       <c r="L35" t="s">
         <v>29</v>
       </c>
-      <c r="M35" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N35" s="1">
+      <c r="M35" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N35" s="2">
         <v>43301</v>
       </c>
       <c r="O35" t="s">
@@ -1389,7 +1108,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16">
       <c r="B36">
         <v>2020</v>
       </c>
@@ -1414,10 +1133,10 @@
       <c r="L36" t="s">
         <v>29</v>
       </c>
-      <c r="M36" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N36" s="1">
+      <c r="M36" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N36" s="2">
         <v>43301</v>
       </c>
       <c r="O36" t="s">
@@ -1427,7 +1146,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16">
       <c r="B37">
         <v>2020</v>
       </c>
@@ -1452,10 +1171,10 @@
       <c r="L37" t="s">
         <v>29</v>
       </c>
-      <c r="M37" s="1">
-        <v>43299</v>
-      </c>
-      <c r="N37" s="1">
+      <c r="M37" s="2">
+        <v>43299</v>
+      </c>
+      <c r="N37" s="2">
         <v>43301</v>
       </c>
       <c r="O37" t="s">
@@ -1465,7 +1184,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16">
       <c r="H38" t="s">
         <v>30</v>
       </c>
@@ -1475,35 +1194,46 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <autoFilter ref="H11:P38"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="70.140625" customWidth="1"/>
-    <col min="10" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" style="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" style="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" style="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" style="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" style="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" style="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" style="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" style="1" width="70.140625" customWidth="1"/>
+    <col min="10" max="11" style="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" style="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" style="1" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>10009</v>
       </c>
@@ -1570,12 +1300,12 @@
         <v>1890324123</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="1">
-        <v>43299</v>
-      </c>
-      <c r="K2" s="1">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2">
+        <v>43299</v>
+      </c>
+      <c r="K2" s="2">
         <v>43301</v>
       </c>
       <c r="L2" t="s">
@@ -1585,7 +1315,7 @@
         <v>-200000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>10009</v>
       </c>
@@ -1611,12 +1341,12 @@
         <v>1890324125</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="1">
-        <v>43299</v>
-      </c>
-      <c r="K3" s="1">
+        <v>31</v>
+      </c>
+      <c r="J3" s="2">
+        <v>43299</v>
+      </c>
+      <c r="K3" s="2">
         <v>43301</v>
       </c>
       <c r="L3" t="s">
@@ -1626,18 +1356,18 @@
         <v>-200000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="M4">
         <f>SUM(M2:M3)</f>
         <v>-400000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -1660,12 +1390,12 @@
         <v>90923</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="1">
-        <v>43299</v>
-      </c>
-      <c r="K5" s="1">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2">
+        <v>43299</v>
+      </c>
+      <c r="K5" s="2">
         <v>43301</v>
       </c>
       <c r="L5" t="s">
@@ -1675,7 +1405,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -1698,12 +1428,12 @@
         <v>90923</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="1">
-        <v>43299</v>
-      </c>
-      <c r="K6" s="1">
+        <v>32</v>
+      </c>
+      <c r="J6" s="2">
+        <v>43299</v>
+      </c>
+      <c r="K6" s="2">
         <v>43301</v>
       </c>
       <c r="L6" t="s">
@@ -1713,7 +1443,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -1736,12 +1466,12 @@
         <v>90923</v>
       </c>
       <c r="I7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="1">
-        <v>43299</v>
-      </c>
-      <c r="K7" s="1">
+        <v>32</v>
+      </c>
+      <c r="J7" s="2">
+        <v>43299</v>
+      </c>
+      <c r="K7" s="2">
         <v>43301</v>
       </c>
       <c r="L7" t="s">
@@ -1751,7 +1481,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -1774,12 +1504,12 @@
         <v>90923</v>
       </c>
       <c r="I8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="1">
-        <v>43299</v>
-      </c>
-      <c r="K8" s="1">
+        <v>32</v>
+      </c>
+      <c r="J8" s="2">
+        <v>43299</v>
+      </c>
+      <c r="K8" s="2">
         <v>43301</v>
       </c>
       <c r="L8" t="s">
@@ -1789,7 +1519,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -1812,12 +1542,12 @@
         <v>90923</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="1">
-        <v>43299</v>
-      </c>
-      <c r="K9" s="1">
+        <v>32</v>
+      </c>
+      <c r="J9" s="2">
+        <v>43299</v>
+      </c>
+      <c r="K9" s="2">
         <v>43301</v>
       </c>
       <c r="L9" t="s">
@@ -1827,7 +1557,7 @@
         <v>-20000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="E10" t="s">
         <v>30</v>
       </c>
@@ -1836,9 +1566,9 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="E11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M11">
         <f>SUM(M10,M4)</f>
@@ -1846,24 +1576,36 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" style="1" width="9.142307692307693"/>
+    <col min="8" max="8" style="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" style="1" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1904,7 +1646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>8</v>
       </c>
@@ -1945,7 +1687,7 @@
         <v>-2000</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>8</v>
       </c>
@@ -1986,7 +1728,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="E4" t="s">
         <v>18</v>
       </c>
@@ -1995,7 +1737,7 @@
         <v>-1000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>3400</v>
       </c>
@@ -2033,7 +1775,7 @@
         <v>-200000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>3400</v>
       </c>
@@ -2071,7 +1813,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>3400</v>
       </c>
@@ -2109,7 +1851,7 @@
         <v>-300000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>3400</v>
       </c>
@@ -2147,7 +1889,7 @@
         <v>-2300</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>3400</v>
       </c>
@@ -2185,7 +1927,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3400</v>
       </c>
@@ -2223,7 +1965,7 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>3400</v>
       </c>
@@ -2261,7 +2003,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>3400</v>
       </c>
@@ -2299,7 +2041,7 @@
         <v>12220</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>3400</v>
       </c>
@@ -2337,7 +2079,7 @@
         <v>32000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>3400</v>
       </c>
@@ -2375,7 +2117,7 @@
         <v>-4000000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>3400</v>
       </c>
@@ -2413,7 +2155,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>3400</v>
       </c>
@@ -2451,7 +2193,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>3400</v>
       </c>
@@ -2489,7 +2231,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>3400</v>
       </c>
@@ -2527,7 +2269,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="E19" t="s">
         <v>27</v>
       </c>
@@ -2536,9 +2278,9 @@
         <v>-4555112</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="E20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M20">
         <f>SUM(M19,M4)</f>
@@ -2546,6 +2288,13 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>